<commit_message>
LoginDDT and addNewCustomer automation codes updated to resolve element not found error and to block spontan ads popup
</commit_message>
<xml_diff>
--- a/src/test/java/com/inetbanking/testData/LoginData1.xlsx
+++ b/src/test/java/com/inetbanking/testData/LoginData1.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\empre\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{E9365DC7-4C5E-4857-9259-66571BF1A636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8373644A-6331-4368-A98B-4762B44CCE14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5784" yWindow="3276" windowWidth="17256" windowHeight="8868"/>
+    <workbookView xWindow="5784" yWindow="3276" windowWidth="17256" windowHeight="8868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>username</t>
   </si>
@@ -50,28 +50,16 @@
     <t>pEnEmam</t>
   </si>
   <si>
-    <t>mngr83460</t>
-  </si>
-  <si>
-    <t>qAbUzyj</t>
-  </si>
-  <si>
-    <t>mngr137319</t>
-  </si>
-  <si>
-    <t>bAdYvyb</t>
-  </si>
-  <si>
-    <t>mngr112909</t>
-  </si>
-  <si>
-    <t>tytUreg</t>
+    <t>mhsZu871</t>
+  </si>
+  <si>
+    <t>pZgbiz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -423,11 +411,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="127" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -460,30 +448,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>